<commit_message>
[update] new data schema, add deps, input facility name
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hkt\mvp\data_populator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hkt\mvp\data_populator\argo-ai-data-populator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35AE68C-FBB3-4A4D-A517-AA3039D91307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC12D69-A4D7-4F2B-91CC-C79EF71978C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="38">
   <si>
     <t>facility</t>
   </si>
@@ -74,9 +74,6 @@
     <t>water_recycled</t>
   </si>
   <si>
-    <t>water_quality</t>
-  </si>
-  <si>
     <t>pest_population_counts</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>soil_pH</t>
-  </si>
-  <si>
     <t>soil_conductivity</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>province</t>
   </si>
   <si>
-    <t>Da Lat</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -134,26 +125,41 @@
     <t>latitude</t>
   </si>
   <si>
-    <t>VHJ6+PH3, Đất, Thôn, Cầu, Xuân Trường, Thành phố Đà Lạt, Lâm Đồng, Vietnam</t>
-  </si>
-  <si>
-    <t>Lam Dong</t>
-  </si>
-  <si>
     <t>plant</t>
   </si>
   <si>
     <t>rice</t>
   </si>
   <si>
-    <t>farm22z</t>
+    <t>soil_moisture_20</t>
+  </si>
+  <si>
+    <t>soil_moisture_40</t>
+  </si>
+  <si>
+    <t>soil_ph</t>
+  </si>
+  <si>
+    <t>Bao Trình, thị trấn Diêm Điền, huyện Thái Thụy, tỉnh Thái Bình</t>
+  </si>
+  <si>
+    <t>Thai Thuy</t>
+  </si>
+  <si>
+    <t>Thai Binh</t>
+  </si>
+  <si>
+    <t>dolphin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -169,6 +175,13 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -192,18 +205,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -417,10 +440,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB892"/>
+  <dimension ref="A1:AC892"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -431,1013 +454,1610 @@
     <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" s="2">
+        <v>45474</v>
+      </c>
+      <c r="I2" s="4">
+        <f ca="1">35+RANDBETWEEN(1,5)</f>
+        <v>38</v>
+      </c>
+      <c r="J2" s="4">
+        <f ca="1">29+RANDBETWEEN(1,3)</f>
+        <v>30</v>
+      </c>
+      <c r="K2" s="1">
+        <f ca="1">RANDBETWEEN(40,60)/10</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1">
+        <v>60</v>
+      </c>
+      <c r="N2" s="1">
+        <v>26.57</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1038.6500000000001</v>
+      </c>
+      <c r="P2" s="1">
+        <v>46.26</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>51.26</v>
+      </c>
+      <c r="R2" s="1">
+        <v>54.26</v>
+      </c>
+      <c r="S2" s="1">
+        <v>26.92</v>
+      </c>
+      <c r="T2" s="1">
+        <v>6.68</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="V2" s="1">
+        <v>597.71</v>
+      </c>
+      <c r="W2" s="1">
+        <v>188.9</v>
+      </c>
+      <c r="X2" s="1">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>7.27</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>402.66</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2">
+        <v>45475</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I17" ca="1" si="0">34+RANDBETWEEN(0,5)</f>
+        <v>36</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J17" ca="1" si="1">29+RANDBETWEEN(1,3)</f>
+        <v>30</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K17" ca="1" si="2">RANDBETWEEN(40,60)/10</f>
+        <v>5.7</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1">
+        <v>57</v>
+      </c>
+      <c r="N3" s="1">
+        <v>45.65</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1047.68</v>
+      </c>
+      <c r="P3" s="1">
+        <v>34.64</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>41.64</v>
+      </c>
+      <c r="R3" s="1">
+        <v>48.64</v>
+      </c>
+      <c r="S3" s="1">
+        <v>23.55</v>
+      </c>
+      <c r="T3" s="1">
+        <v>7.24</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="V3" s="1">
+        <v>636.28</v>
+      </c>
+      <c r="W3" s="1">
+        <v>130.9</v>
+      </c>
+      <c r="X3" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>368.22</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E4" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2">
+        <v>45476</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1">
+        <v>50</v>
+      </c>
+      <c r="N4" s="1">
+        <v>11.54</v>
+      </c>
+      <c r="O4" s="1">
+        <v>979.72</v>
+      </c>
+      <c r="P4" s="1">
+        <v>54.2</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>57.2</v>
+      </c>
+      <c r="R4" s="1">
+        <v>63.2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="T4" s="1">
+        <v>6.71</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="V4" s="1">
+        <v>399.34</v>
+      </c>
+      <c r="W4" s="1">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="X4" s="1">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>2.87</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>4.71</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>373.62</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>2.63</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E5" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2">
+        <v>45477</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="1">
+        <v>58</v>
+      </c>
+      <c r="N5" s="1">
+        <v>51.33</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1050.0899999999999</v>
+      </c>
+      <c r="P5" s="1">
+        <v>54.64</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>61.64</v>
+      </c>
+      <c r="R5" s="1">
+        <v>65.64</v>
+      </c>
+      <c r="S5" s="1">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="T5" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="V5" s="1">
+        <v>239.32</v>
+      </c>
+      <c r="W5" s="1">
+        <v>59.9</v>
+      </c>
+      <c r="X5" s="1">
+        <v>50</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>5.83</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>409.62</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>2.44</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E6" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2">
+        <v>45478</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" ca="1" si="1"/>
         <v>31</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="K6" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="1">
+        <v>42</v>
+      </c>
+      <c r="N6" s="1">
+        <v>56.95</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1024.55</v>
+      </c>
+      <c r="P6" s="1">
+        <v>23.54</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>25.54</v>
+      </c>
+      <c r="R6" s="1">
+        <v>29.54</v>
+      </c>
+      <c r="S6" s="1">
+        <v>19.48</v>
+      </c>
+      <c r="T6" s="1">
+        <v>5.74</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="V6" s="1">
+        <v>496.34</v>
+      </c>
+      <c r="W6" s="1">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="X6" s="1">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>7.83</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>407.3</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E7" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="2">
+        <v>45479</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="L7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1">
+        <v>58</v>
+      </c>
+      <c r="N7" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1036.8599999999999</v>
+      </c>
+      <c r="P7" s="1">
+        <v>34.35</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>37.35</v>
+      </c>
+      <c r="R7" s="1">
+        <v>39.35</v>
+      </c>
+      <c r="S7" s="1">
+        <v>29.12</v>
+      </c>
+      <c r="T7" s="1">
+        <v>5.68</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="V7" s="1">
+        <v>275.58999999999997</v>
+      </c>
+      <c r="W7" s="1">
+        <v>60.1</v>
+      </c>
+      <c r="X7" s="1">
         <v>15</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Y7" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>439.62</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>7.54</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2">
+        <v>45480</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.6</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="1">
+        <v>50</v>
+      </c>
+      <c r="N8" s="1">
+        <v>10.39</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1046.18</v>
+      </c>
+      <c r="P8" s="1">
+        <v>27.08</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>30.08</v>
+      </c>
+      <c r="R8" s="1">
+        <v>34.08</v>
+      </c>
+      <c r="S8" s="1">
+        <v>23.56</v>
+      </c>
+      <c r="T8" s="1">
+        <v>6.58</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="V8" s="1">
+        <v>804.92</v>
+      </c>
+      <c r="W8" s="1">
+        <v>185.1</v>
+      </c>
+      <c r="X8" s="1">
+        <v>61</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>6.89</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>310.62</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2">
+        <v>45481</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="1">
+        <v>59</v>
+      </c>
+      <c r="N9" s="1">
+        <v>78.180000000000007</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1050.4000000000001</v>
+      </c>
+      <c r="P9" s="1">
+        <v>38.57</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>40.57</v>
+      </c>
+      <c r="R9" s="1">
+        <v>41.57</v>
+      </c>
+      <c r="S9" s="1">
+        <v>20.51</v>
+      </c>
+      <c r="T9" s="1">
+        <v>5.67</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="V9" s="1">
+        <v>243.02</v>
+      </c>
+      <c r="W9" s="1">
+        <v>55.8</v>
+      </c>
+      <c r="X9" s="1">
+        <v>37</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>7.96</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>340.94</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>6.67</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2">
+        <v>45482</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.8</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1">
+        <v>60</v>
+      </c>
+      <c r="N10" s="1">
+        <v>75.78</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1045.17</v>
+      </c>
+      <c r="P10" s="1">
+        <v>23.64</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>24.64</v>
+      </c>
+      <c r="R10" s="1">
+        <v>30.64</v>
+      </c>
+      <c r="S10" s="1">
+        <v>29.94</v>
+      </c>
+      <c r="T10" s="1">
+        <v>6.89</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="V10" s="1">
+        <v>489.34</v>
+      </c>
+      <c r="W10" s="1">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="X10" s="1">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>2.48</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>313.33999999999997</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>1.88</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="2">
+        <v>45483</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.8</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="1">
+        <v>59</v>
+      </c>
+      <c r="N11" s="1">
+        <v>6.92</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1045.02</v>
+      </c>
+      <c r="P11" s="1">
+        <v>25.29</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>31.29</v>
+      </c>
+      <c r="R11" s="1">
+        <v>33.29</v>
+      </c>
+      <c r="S11" s="1">
+        <v>21.24</v>
+      </c>
+      <c r="T11" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="V11" s="1">
+        <v>930.16</v>
+      </c>
+      <c r="W11" s="1">
+        <v>220.6</v>
+      </c>
+      <c r="X11" s="1">
+        <v>51</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>301.79000000000002</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E12" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2">
+        <v>45484</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="1">
+        <v>56</v>
+      </c>
+      <c r="N12" s="1">
+        <v>63.91</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1005.88</v>
+      </c>
+      <c r="P12" s="1">
+        <v>43.95</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>44.95</v>
+      </c>
+      <c r="R12" s="1">
+        <v>45.95</v>
+      </c>
+      <c r="S12" s="1">
+        <v>28.16</v>
+      </c>
+      <c r="T12" s="1">
+        <v>6.37</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="V12" s="1">
+        <v>485.7</v>
+      </c>
+      <c r="W12" s="1">
+        <v>107.6</v>
+      </c>
+      <c r="X12" s="1">
+        <v>90</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>2.39</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>473.29</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>7.41</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2">
+        <v>45485</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="1">
+        <v>57</v>
+      </c>
+      <c r="N13" s="1">
+        <v>85.08</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1050.96</v>
+      </c>
+      <c r="P13" s="1">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="R13" s="1">
+        <v>42.7</v>
+      </c>
+      <c r="S13" s="1">
+        <v>27.14</v>
+      </c>
+      <c r="T13" s="1">
+        <v>5.66</v>
+      </c>
+      <c r="U13" s="1">
+        <v>1.36</v>
+      </c>
+      <c r="V13" s="1">
+        <v>984.67</v>
+      </c>
+      <c r="W13" s="1">
+        <v>309.60000000000002</v>
+      </c>
+      <c r="X13" s="1">
+        <v>78</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>6.61</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>3.62</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>394.44</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>7.93</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="2">
+        <v>45486</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="1">
+        <v>44</v>
+      </c>
+      <c r="N14" s="1">
+        <v>33.93</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1016.71</v>
+      </c>
+      <c r="P14" s="1">
+        <v>32.909999999999997</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="R14" s="1">
+        <v>44.91</v>
+      </c>
+      <c r="S14" s="1">
+        <v>21.04</v>
+      </c>
+      <c r="T14" s="1">
+        <v>6.93</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V14" s="1">
+        <v>749.45</v>
+      </c>
+      <c r="W14" s="1">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="X14" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>3.01</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>426.1</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>1.63</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E15" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="2">
+        <v>45487</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="1">
+        <v>47</v>
+      </c>
+      <c r="N15" s="1">
+        <v>67.37</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1028.49</v>
+      </c>
+      <c r="P15" s="1">
+        <v>38.29</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>42.29</v>
+      </c>
+      <c r="R15" s="1">
+        <v>46.29</v>
+      </c>
+      <c r="S15" s="1">
+        <v>17.71</v>
+      </c>
+      <c r="T15" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="V15" s="1">
+        <v>275.25</v>
+      </c>
+      <c r="W15" s="1">
+        <v>82.2</v>
+      </c>
+      <c r="X15" s="1">
+        <v>61</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>437.59</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>6.27</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E16" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2">
+        <v>45488</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.7</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="M16" s="1">
+        <v>52</v>
+      </c>
+      <c r="N16" s="1">
+        <v>18.41</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1011.97</v>
+      </c>
+      <c r="P16" s="1">
+        <v>18.43</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>21.43</v>
+      </c>
+      <c r="R16" s="1">
+        <v>26.43</v>
+      </c>
+      <c r="S16" s="1">
+        <v>15.55</v>
+      </c>
+      <c r="T16" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="U16" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="V16" s="1">
+        <v>727.85</v>
+      </c>
+      <c r="W16" s="1">
+        <v>189.2</v>
+      </c>
+      <c r="X16" s="1">
+        <v>50</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>2.33</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>3.72</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>397.49</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D17" s="1">
+        <v>106.56213138823</v>
+      </c>
+      <c r="E17" s="1">
+        <v>20.564662101784901</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="2">
+        <v>45489</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" ca="1" si="1"/>
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F2" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G2" s="2">
-        <v>45474</v>
-      </c>
-      <c r="H2" s="1">
-        <v>27.49</v>
-      </c>
-      <c r="I2" s="1">
-        <v>10.47</v>
-      </c>
-      <c r="J2" s="1">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1">
-        <v>65.16</v>
-      </c>
-      <c r="M2" s="1">
-        <v>77.709999999999994</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1002.02</v>
-      </c>
-      <c r="O2" s="1">
-        <v>14.35</v>
-      </c>
-      <c r="P2" s="1">
-        <v>26.69</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>6.93</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="S2" s="1">
-        <v>887.23</v>
-      </c>
-      <c r="T2" s="1">
-        <v>368.76</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="V2" s="1">
-        <v>48</v>
-      </c>
-      <c r="W2" s="1">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="X2" s="1">
-        <v>1.22</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>411.56</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>9.85</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F3" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G3" s="2">
-        <v>45475</v>
-      </c>
-      <c r="H3" s="1">
-        <v>39.01</v>
-      </c>
-      <c r="I3" s="1">
-        <v>19.55</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1.26</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="1">
-        <v>82.82</v>
-      </c>
-      <c r="M3" s="1">
-        <v>55.84</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1035.22</v>
-      </c>
-      <c r="O3" s="1">
-        <v>36.86</v>
-      </c>
-      <c r="P3" s="1">
-        <v>19.59</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>6.63</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1.03</v>
-      </c>
-      <c r="S3" s="1">
-        <v>576.04</v>
-      </c>
-      <c r="T3" s="1">
-        <v>426.66</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="V3" s="1">
+      <c r="K17" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.3</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="1">
+        <v>41</v>
+      </c>
+      <c r="N17" s="1">
+        <v>82.13</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1050.4100000000001</v>
+      </c>
+      <c r="P17" s="1">
+        <v>55.25</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>59.25</v>
+      </c>
+      <c r="R17" s="1">
+        <v>64.25</v>
+      </c>
+      <c r="S17" s="1">
+        <v>20.73</v>
+      </c>
+      <c r="T17" s="1">
+        <v>5.97</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="V17" s="1">
+        <v>618.86</v>
+      </c>
+      <c r="W17" s="1">
+        <v>178.2</v>
+      </c>
+      <c r="X17" s="1">
         <v>50</v>
       </c>
-      <c r="W3" s="1">
-        <v>9.34</v>
-      </c>
-      <c r="X3" s="1">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>446.13</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>3.15</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F4" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G4" s="2">
-        <v>45476</v>
-      </c>
-      <c r="H4" s="1">
-        <v>34.64</v>
-      </c>
-      <c r="I4" s="1">
-        <v>14.72</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2.42</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="1">
-        <v>72.930000000000007</v>
-      </c>
-      <c r="M4" s="1">
-        <v>42.42</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1005.19</v>
-      </c>
-      <c r="O4" s="1">
-        <v>39.340000000000003</v>
-      </c>
-      <c r="P4" s="1">
-        <v>20.23</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>7.15</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="S4" s="1">
-        <v>945.16</v>
-      </c>
-      <c r="T4" s="1">
-        <v>363.86</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="V4" s="1">
-        <v>95</v>
-      </c>
-      <c r="W4" s="1">
-        <v>3.16</v>
-      </c>
-      <c r="X4" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>393.04</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F5" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G5" s="2">
-        <v>45477</v>
-      </c>
-      <c r="H5" s="1">
-        <v>31.97</v>
-      </c>
-      <c r="I5" s="1">
-        <v>17.63</v>
-      </c>
-      <c r="J5" s="1">
-        <v>13.48</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="1">
-        <v>48.15</v>
-      </c>
-      <c r="M5" s="1">
-        <v>90.64</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1006.09</v>
-      </c>
-      <c r="O5" s="1">
-        <v>47.27</v>
-      </c>
-      <c r="P5" s="1">
-        <v>14.14</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>5.96</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1.38</v>
-      </c>
-      <c r="S5" s="1">
-        <v>818.9</v>
-      </c>
-      <c r="T5" s="1">
-        <v>356.06</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0.63</v>
-      </c>
-      <c r="V5" s="1">
-        <v>35</v>
-      </c>
-      <c r="W5" s="1">
-        <v>5.07</v>
-      </c>
-      <c r="X5" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>312.02999999999997</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>2.09</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F6" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G6" s="2">
-        <v>45478</v>
-      </c>
-      <c r="H6" s="1">
-        <v>23.12</v>
-      </c>
-      <c r="I6" s="1">
-        <v>23.61</v>
-      </c>
-      <c r="J6" s="1">
-        <v>9.1</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="1">
-        <v>43.53</v>
-      </c>
-      <c r="M6" s="1">
-        <v>11.12</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1037.67</v>
-      </c>
-      <c r="O6" s="1">
-        <v>31.58</v>
-      </c>
-      <c r="P6" s="1">
-        <v>13.63</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>6.23</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0.69</v>
-      </c>
-      <c r="S6" s="1">
-        <v>998.14</v>
-      </c>
-      <c r="T6" s="1">
-        <v>328.38</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1.19</v>
-      </c>
-      <c r="V6" s="1">
-        <v>97</v>
-      </c>
-      <c r="W6" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="X6" s="1">
-        <v>1.76</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>412.46</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>3.73</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F7" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G7" s="2">
-        <v>45479</v>
-      </c>
-      <c r="H7" s="1">
-        <v>36.979999999999997</v>
-      </c>
-      <c r="I7" s="1">
-        <v>14.26</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3.73</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="1">
-        <v>87.45</v>
-      </c>
-      <c r="M7" s="1">
-        <v>32.67</v>
-      </c>
-      <c r="N7" s="1">
-        <v>988.69</v>
-      </c>
-      <c r="O7" s="1">
-        <v>25.16</v>
-      </c>
-      <c r="P7" s="1">
-        <v>27.27</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>6.25</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="S7" s="1">
-        <v>956.64</v>
-      </c>
-      <c r="T7" s="1">
-        <v>343.82</v>
-      </c>
-      <c r="U7" s="1">
-        <v>0.91</v>
-      </c>
-      <c r="V7" s="1">
-        <v>23</v>
-      </c>
-      <c r="W7" s="1">
-        <v>2.92</v>
-      </c>
-      <c r="X7" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>324.37</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>6.26</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F8" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G8" s="2">
-        <v>45480</v>
-      </c>
-      <c r="H8" s="1">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="I8" s="1">
-        <v>14.12</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="1">
-        <v>53.58</v>
-      </c>
-      <c r="M8" s="1">
-        <v>29.5</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1018.37</v>
-      </c>
-      <c r="O8" s="1">
-        <v>30.26</v>
-      </c>
-      <c r="P8" s="1">
-        <v>22.22</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>7.43</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="S8" s="1">
-        <v>573.79</v>
-      </c>
-      <c r="T8" s="1">
-        <v>161.96</v>
-      </c>
-      <c r="U8" s="1">
-        <v>0.51</v>
-      </c>
-      <c r="V8" s="1">
-        <v>22</v>
-      </c>
-      <c r="W8" s="1">
-        <v>3.36</v>
-      </c>
-      <c r="X8" s="1">
-        <v>3.37</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>495.73</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F9" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G9" s="2">
-        <v>45481</v>
-      </c>
-      <c r="H9" s="1">
-        <v>27.56</v>
-      </c>
-      <c r="I9" s="1">
-        <v>13.95</v>
-      </c>
-      <c r="J9" s="1">
-        <v>9.36</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="1">
-        <v>52.89</v>
-      </c>
-      <c r="M9" s="1">
-        <v>53.67</v>
-      </c>
-      <c r="N9" s="1">
-        <v>1003.65</v>
-      </c>
-      <c r="O9" s="1">
-        <v>41.41</v>
-      </c>
-      <c r="P9" s="1">
-        <v>33.53</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>5.88</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="S9" s="1">
-        <v>705.71</v>
-      </c>
-      <c r="T9" s="1">
-        <v>205.21</v>
-      </c>
-      <c r="U9" s="1">
-        <v>1.27</v>
-      </c>
-      <c r="V9" s="1">
-        <v>21</v>
-      </c>
-      <c r="W9" s="1">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="X9" s="1">
-        <v>3.45</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>300.97000000000003</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>7.84</v>
-      </c>
-      <c r="AA9" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F10" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G10" s="2">
-        <v>45482</v>
-      </c>
-      <c r="H10" s="1">
-        <v>32.89</v>
-      </c>
-      <c r="I10" s="1">
-        <v>14.4</v>
-      </c>
-      <c r="J10" s="1">
-        <v>14.82</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="1">
-        <v>58.63</v>
-      </c>
-      <c r="M10" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="N10" s="1">
-        <v>967.34</v>
-      </c>
-      <c r="O10" s="1">
-        <v>52.72</v>
-      </c>
-      <c r="P10" s="1">
-        <v>14.9</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>6.93</v>
-      </c>
-      <c r="R10" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="S10" s="1">
-        <v>188</v>
-      </c>
-      <c r="T10" s="1">
-        <v>187.21</v>
-      </c>
-      <c r="U10" s="1">
-        <v>1.38</v>
-      </c>
-      <c r="V10" s="1">
-        <v>92</v>
-      </c>
-      <c r="W10" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="X10" s="1">
-        <v>3.71</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>358.91</v>
-      </c>
-      <c r="Z10" s="1">
-        <v>4.41</v>
-      </c>
-      <c r="AA10" s="1">
-        <v>0.52</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="1">
-        <v>108.561573082241</v>
-      </c>
-      <c r="F11" s="1">
-        <v>11.8819075448256</v>
-      </c>
-      <c r="G11" s="2">
-        <v>45483</v>
-      </c>
-      <c r="H11" s="1">
-        <v>26.06</v>
-      </c>
-      <c r="I11" s="1">
-        <v>14.55</v>
-      </c>
-      <c r="J11" s="1">
-        <v>5.22</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="1">
-        <v>53.2</v>
-      </c>
-      <c r="M11" s="1">
-        <v>95.14</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1008.01</v>
-      </c>
-      <c r="O11" s="1">
-        <v>32.56</v>
-      </c>
-      <c r="P11" s="1">
-        <v>22.92</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>6.53</v>
-      </c>
-      <c r="R11" s="1">
-        <v>1.46</v>
-      </c>
-      <c r="S11" s="1">
-        <v>626.22</v>
-      </c>
-      <c r="T11" s="1">
-        <v>70.260000000000005</v>
-      </c>
-      <c r="U11" s="1">
-        <v>1.45</v>
-      </c>
-      <c r="V11" s="1">
-        <v>71</v>
-      </c>
-      <c r="W11" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="X11" s="1">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>371.2</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>5.74</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Y17" s="1">
+        <v>2.73</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>365.33</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>7.48</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -4022,6 +4642,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="H1:H17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>